<commit_message>
Afegint dades imatges de linyola
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Baptismes/Excel/Index_llibres_Baptismes.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Baptismes/Excel/Index_llibres_Baptismes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7B169E-C169-40E2-8CD6-32D690D5B98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA63C9E-D2A3-4F95-B729-85FFBF9D9A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="560">
   <si>
     <t>Cognoms</t>
   </si>
@@ -115,7 +115,16 @@
     <t>Mestre de Cases</t>
   </si>
   <si>
+    <t>Ferrer</t>
+  </si>
+  <si>
     <t>Maria Novell</t>
+  </si>
+  <si>
+    <t>Paula Pedrós</t>
+  </si>
+  <si>
+    <t>Fuster</t>
   </si>
   <si>
     <t>23/03/1770</t>
@@ -131,6 +140,9 @@
   </si>
   <si>
     <t>Josep Solé (Pages)</t>
+  </si>
+  <si>
+    <t>14/01/1801</t>
   </si>
   <si>
     <t>U.D. U.I.</t>
@@ -1407,6 +1419,339 @@
   <si>
     <t>Torrent Cascalló Maria Antonia</t>
   </si>
+  <si>
+    <t>Gertrudis Bonjorn</t>
+  </si>
+  <si>
+    <t>03-0123</t>
+  </si>
+  <si>
+    <t>03-0122 - 03-0123</t>
+  </si>
+  <si>
+    <t>120 , 121</t>
+  </si>
+  <si>
+    <t>¿? Bonjorn Anton Joseph Fransisco</t>
+  </si>
+  <si>
+    <t>Anton Vallés (Pages)</t>
+  </si>
+  <si>
+    <t>Antonia Oriola</t>
+  </si>
+  <si>
+    <t>14/11/1794</t>
+  </si>
+  <si>
+    <t>Miquel Majoral (Mestre de Cases)</t>
+  </si>
+  <si>
+    <t>Pares Incognits Anna Maria</t>
+  </si>
+  <si>
+    <t>INCOGNIT</t>
+  </si>
+  <si>
+    <t>Pedrós Duart Manuel Ignasi Pau</t>
+  </si>
+  <si>
+    <t>08/11/1794</t>
+  </si>
+  <si>
+    <t>Joseph Pedrós</t>
+  </si>
+  <si>
+    <t>Maria Duart</t>
+  </si>
+  <si>
+    <t>Bonaventura Alexandre</t>
+  </si>
+  <si>
+    <t>01/12/1794</t>
+  </si>
+  <si>
+    <t>Gregori Gilavert</t>
+  </si>
+  <si>
+    <t>Gilavert Roma Maria Antonia Paula</t>
+  </si>
+  <si>
+    <t>Rosa Roma</t>
+  </si>
+  <si>
+    <t>30/11/1794</t>
+  </si>
+  <si>
+    <t>Joseph Giné (Pages)</t>
+  </si>
+  <si>
+    <t>Antonia ¿? Valles</t>
+  </si>
+  <si>
+    <t>Mas Castelló Domingo Joseph Pau</t>
+  </si>
+  <si>
+    <t>05/12/1794</t>
+  </si>
+  <si>
+    <t>Anton Mas</t>
+  </si>
+  <si>
+    <t>Francesca Castelló</t>
+  </si>
+  <si>
+    <t>Domingo Mas (Pages)</t>
+  </si>
+  <si>
+    <t>06/12/1794</t>
+  </si>
+  <si>
+    <t>Domingo Massot</t>
+  </si>
+  <si>
+    <t>Raimunda Massot</t>
+  </si>
+  <si>
+    <t>Ribes Vergé Antonia Ramunda</t>
+  </si>
+  <si>
+    <t>16/12/1794</t>
+  </si>
+  <si>
+    <t>Jaume Codina</t>
+  </si>
+  <si>
+    <t>Maria Xandre</t>
+  </si>
+  <si>
+    <t>15/12/1794</t>
+  </si>
+  <si>
+    <t>Ramon Vergé Mas (Pages)</t>
+  </si>
+  <si>
+    <t>Maria Rosa Sunyé</t>
+  </si>
+  <si>
+    <t>Codina Xandre Ramon Anton Pau</t>
+  </si>
+  <si>
+    <t>17/12/1794</t>
+  </si>
+  <si>
+    <t>Domingo Mas</t>
+  </si>
+  <si>
+    <t>Maria Cerret?</t>
+  </si>
+  <si>
+    <t>Magdalena Mas</t>
+  </si>
+  <si>
+    <t>Mas Cerret? Magdalena Antonia</t>
+  </si>
+  <si>
+    <t>20/12/1794</t>
+  </si>
+  <si>
+    <t>Joan Arnau</t>
+  </si>
+  <si>
+    <t>Quiteria Falcó</t>
+  </si>
+  <si>
+    <t>19/12/1794</t>
+  </si>
+  <si>
+    <t>Fransisco Oriola (Pages)</t>
+  </si>
+  <si>
+    <t>Maria Giné</t>
+  </si>
+  <si>
+    <t>Arnau Falcó Fransisco Joseph Pau</t>
+  </si>
+  <si>
+    <t>03-0158</t>
+  </si>
+  <si>
+    <t>Marti Jovells Antonia Maria Joana</t>
+  </si>
+  <si>
+    <t>09/01/1801</t>
+  </si>
+  <si>
+    <t>08/01/1801</t>
+  </si>
+  <si>
+    <t>Fransisco Jovells (Casat)(El Masó)</t>
+  </si>
+  <si>
+    <t>Antonia Mas Martí</t>
+  </si>
+  <si>
+    <t>Antonio Martí i Antonia Mas</t>
+  </si>
+  <si>
+    <t>Jaume Jovells (Golmés) i Francisca Felip (Anglesola)</t>
+  </si>
+  <si>
+    <t>Joan Martí Mas</t>
+  </si>
+  <si>
+    <t>Fransisca Jovells Felip</t>
+  </si>
+  <si>
+    <t>Caelles Ganyet Ramon Pau Joan</t>
+  </si>
+  <si>
+    <t>15/01/1801</t>
+  </si>
+  <si>
+    <t>Cecilia Sol (Donsella)</t>
+  </si>
+  <si>
+    <t>Ramon Duch (Fadri)</t>
+  </si>
+  <si>
+    <t>Joan Caelles (Llenera) i Serafina Begardit (La Molsora)</t>
+  </si>
+  <si>
+    <t>Antonio Ganyet i Josepha Solé (aquesta de Fondarella)</t>
+  </si>
+  <si>
+    <t>Valentí Caelles Begardit</t>
+  </si>
+  <si>
+    <t>Helena Ganyet Solé</t>
+  </si>
+  <si>
+    <t>Pedrós Duart Rosa Maria Antonia</t>
+  </si>
+  <si>
+    <t>26/01/1801</t>
+  </si>
+  <si>
+    <t>Antonio Vallés</t>
+  </si>
+  <si>
+    <t>Rosa Alexandre</t>
+  </si>
+  <si>
+    <t>Ignasi Pedrós i Llucia Mas</t>
+  </si>
+  <si>
+    <t>Josep Pedrós Mas</t>
+  </si>
+  <si>
+    <t>Mariano Duart i Magdalena Alexandre</t>
+  </si>
+  <si>
+    <t>Maria Duart Alexandre</t>
+  </si>
+  <si>
+    <t>Civit Batlle Rosa Teresa Antonia</t>
+  </si>
+  <si>
+    <t>31/01/1801</t>
+  </si>
+  <si>
+    <t>30/01/1801</t>
+  </si>
+  <si>
+    <t>Fransisco Trepat</t>
+  </si>
+  <si>
+    <t>Rosa Solé</t>
+  </si>
+  <si>
+    <t>Josep Civit i Paula Serra</t>
+  </si>
+  <si>
+    <t>Josep Civit Serra</t>
+  </si>
+  <si>
+    <t>Pau Batlle i Cecilia Vergé</t>
+  </si>
+  <si>
+    <t>Antonia Batlle Vergé</t>
+  </si>
+  <si>
+    <t>Pedrós Boldú Antonio Ramon Joan</t>
+  </si>
+  <si>
+    <t>06/02/1801</t>
+  </si>
+  <si>
+    <t>05/02/1801</t>
+  </si>
+  <si>
+    <t>Antonio Boldu</t>
+  </si>
+  <si>
+    <t>Josep Pedros i Paula Felip</t>
+  </si>
+  <si>
+    <t>Bonaventura Boldú i Maria Badía (Aquesta de Miralcamp)</t>
+  </si>
+  <si>
+    <t>Ignasi Pedrós Felip</t>
+  </si>
+  <si>
+    <t>Maria Boldú Badía</t>
+  </si>
+  <si>
+    <t>Bergadà Civit Quiteria Raimunda Joana</t>
+  </si>
+  <si>
+    <t>17/02/1801</t>
+  </si>
+  <si>
+    <t>16/02/1801</t>
+  </si>
+  <si>
+    <t>Ramón Falcó</t>
+  </si>
+  <si>
+    <t>Josep Bergadà i Mariangela Ros</t>
+  </si>
+  <si>
+    <t>Josep Civit i Teresa Torrent</t>
+  </si>
+  <si>
+    <t>Cecilia Civit Torrent</t>
+  </si>
+  <si>
+    <t>Jaume Bergadà Ros</t>
+  </si>
+  <si>
+    <t>Margall Fusté Ramon Josep Joan</t>
+  </si>
+  <si>
+    <t>22/02/1801</t>
+  </si>
+  <si>
+    <t>Jaume Margall</t>
+  </si>
+  <si>
+    <t>Maria Fusté</t>
+  </si>
+  <si>
+    <t>21/02/1801</t>
+  </si>
+  <si>
+    <t>Ramon Torrent Mas</t>
+  </si>
+  <si>
+    <t>Maria Folguera (Bellcaire)</t>
+  </si>
+  <si>
+    <t>Fransisco Margall i Helena Mas</t>
+  </si>
+  <si>
+    <t>Felip Fusté (de Bellcaire) i Maria Folguera (Castellserà)</t>
+  </si>
 </sst>
 </file>
 
@@ -1915,8 +2260,8 @@
   <dimension ref="A1:Q17779"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1947,13 +2292,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1989,21 +2334,21 @@
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D2" s="25">
         <v>3</v>
@@ -2012,35 +2357,35 @@
         <v>1770</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2" s="8"/>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O2"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D3" s="25">
         <v>3</v>
@@ -2049,37 +2394,37 @@
         <v>1770</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O3"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D4" s="25">
         <v>3</v>
@@ -2088,37 +2433,37 @@
         <v>1770</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
         <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" t="s">
-        <v>36</v>
       </c>
       <c r="O4"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5" s="25">
         <v>3</v>
@@ -2127,37 +2472,37 @@
         <v>1770</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" t="s">
         <v>47</v>
-      </c>
-      <c r="M5" t="s">
-        <v>48</v>
-      </c>
-      <c r="N5" t="s">
-        <v>43</v>
       </c>
       <c r="O5"/>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" s="25">
         <v>3</v>
@@ -2166,76 +2511,76 @@
         <v>1770</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="N6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O6"/>
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E7">
         <v>1770</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7" s="8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" t="s">
         <v>59</v>
-      </c>
-      <c r="M7" t="s">
-        <v>60</v>
-      </c>
-      <c r="N7" t="s">
-        <v>55</v>
       </c>
       <c r="O7"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D8" s="25">
         <v>4</v>
@@ -2244,37 +2589,37 @@
         <v>1770</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" t="s">
         <v>67</v>
-      </c>
-      <c r="N8" t="s">
-        <v>63</v>
       </c>
       <c r="O8"/>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D9" s="25">
         <v>4</v>
@@ -2283,37 +2628,37 @@
         <v>1770</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" t="s">
         <v>74</v>
-      </c>
-      <c r="N9" t="s">
-        <v>70</v>
       </c>
       <c r="O9"/>
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D10" s="25">
         <v>4</v>
@@ -2322,37 +2667,37 @@
         <v>1770</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10" s="8" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="M10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O10"/>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D11" s="25">
         <v>4</v>
@@ -2361,40 +2706,40 @@
         <v>1770</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="L11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="M11" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" t="s">
         <v>88</v>
-      </c>
-      <c r="N11" t="s">
-        <v>84</v>
       </c>
       <c r="O11"/>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E12">
         <v>1770</v>
@@ -2408,19 +2753,19 @@
       <c r="L12"/>
       <c r="M12"/>
       <c r="N12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O12"/>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D13" s="25">
         <v>13</v>
@@ -2429,35 +2774,35 @@
         <v>1771</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13" s="8"/>
       <c r="L13" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="M13" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="N13"/>
       <c r="O13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D14" s="25">
         <v>13</v>
@@ -2466,25 +2811,25 @@
         <v>1771</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="L14" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="M14" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="N14" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O14" t="s">
         <v>12</v>
@@ -2492,13 +2837,13 @@
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D15" s="25">
         <v>13</v>
@@ -2507,25 +2852,25 @@
         <v>1771</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15" s="8" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="L15" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M15" t="s">
+        <v>112</v>
+      </c>
+      <c r="N15" t="s">
         <v>108</v>
-      </c>
-      <c r="N15" t="s">
-        <v>104</v>
       </c>
       <c r="O15" t="s">
         <v>12</v>
@@ -2533,13 +2878,13 @@
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D16" s="25">
         <v>13</v>
@@ -2548,25 +2893,25 @@
         <v>1771</v>
       </c>
       <c r="F16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L16" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" t="s">
+        <v>120</v>
+      </c>
+      <c r="N16" t="s">
         <v>115</v>
-      </c>
-      <c r="M16" t="s">
-        <v>116</v>
-      </c>
-      <c r="N16" t="s">
-        <v>111</v>
       </c>
       <c r="O16" t="s">
         <v>12</v>
@@ -2574,13 +2919,13 @@
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D17" s="25">
         <v>13</v>
@@ -2589,25 +2934,25 @@
         <v>1771</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17" s="8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="L17" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" t="s">
         <v>122</v>
-      </c>
-      <c r="M17" t="s">
-        <v>123</v>
-      </c>
-      <c r="N17" t="s">
-        <v>118</v>
       </c>
       <c r="O17" t="s">
         <v>12</v>
@@ -2615,13 +2960,13 @@
     </row>
     <row r="18" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D18" s="25">
         <v>20</v>
@@ -2630,25 +2975,25 @@
         <v>1773</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18" s="28" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="L18" t="s">
+        <v>134</v>
+      </c>
+      <c r="M18" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18" t="s">
         <v>130</v>
-      </c>
-      <c r="M18" t="s">
-        <v>131</v>
-      </c>
-      <c r="N18" t="s">
-        <v>126</v>
       </c>
       <c r="O18" t="s">
         <v>12</v>
@@ -2656,13 +3001,13 @@
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D19" s="25">
         <v>20</v>
@@ -2671,25 +3016,25 @@
         <v>1773</v>
       </c>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G19" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19" s="8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="L19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M19" t="s">
+        <v>141</v>
+      </c>
+      <c r="N19" t="s">
         <v>137</v>
-      </c>
-      <c r="N19" t="s">
-        <v>133</v>
       </c>
       <c r="O19" t="s">
         <v>12</v>
@@ -2697,13 +3042,13 @@
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D20" s="25">
         <v>20</v>
@@ -2712,25 +3057,25 @@
         <v>1773</v>
       </c>
       <c r="F20" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G20" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20" s="28" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="L20" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M20" t="s">
+        <v>147</v>
+      </c>
+      <c r="N20" t="s">
         <v>143</v>
-      </c>
-      <c r="N20" t="s">
-        <v>139</v>
       </c>
       <c r="O20" t="s">
         <v>12</v>
@@ -2738,13 +3083,13 @@
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D21" s="25">
         <v>20</v>
@@ -2753,25 +3098,25 @@
         <v>1773</v>
       </c>
       <c r="F21" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21" s="8" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="L21" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="M21" t="s">
+        <v>153</v>
+      </c>
+      <c r="N21" t="s">
         <v>149</v>
-      </c>
-      <c r="N21" t="s">
-        <v>145</v>
       </c>
       <c r="O21" t="s">
         <v>12</v>
@@ -2779,13 +3124,13 @@
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D22" s="25">
         <v>20</v>
@@ -2794,25 +3139,25 @@
         <v>1773</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22" s="28" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L22" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="M22" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N22" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O22" t="s">
         <v>12</v>
@@ -2820,13 +3165,13 @@
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D23" s="25">
         <v>20</v>
@@ -2835,25 +3180,25 @@
         <v>1773</v>
       </c>
       <c r="F23" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23" s="8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="L23" t="s">
+        <v>162</v>
+      </c>
+      <c r="M23" t="s">
+        <v>163</v>
+      </c>
+      <c r="N23" t="s">
         <v>158</v>
-      </c>
-      <c r="M23" t="s">
-        <v>159</v>
-      </c>
-      <c r="N23" t="s">
-        <v>154</v>
       </c>
       <c r="O23" t="s">
         <v>13</v>
@@ -2861,13 +3206,13 @@
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D24" s="25">
         <v>28</v>
@@ -2876,25 +3221,25 @@
         <v>1774</v>
       </c>
       <c r="F24" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G24" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="L24" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="M24" t="s">
+        <v>169</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="O24" t="s">
         <v>12</v>
@@ -2902,13 +3247,13 @@
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D25" s="25">
         <v>28</v>
@@ -2917,25 +3262,25 @@
         <v>1774</v>
       </c>
       <c r="F25" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G25" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25" s="8" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="L25" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="M25" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="N25" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="O25" t="s">
         <v>12</v>
@@ -2943,13 +3288,13 @@
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D26" s="25">
         <v>28</v>
@@ -2958,25 +3303,25 @@
         <v>1774</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="L26" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M26" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="N26" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="O26" t="s">
         <v>12</v>
@@ -2984,13 +3329,13 @@
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D27" s="25">
         <v>28</v>
@@ -2999,25 +3344,25 @@
         <v>1774</v>
       </c>
       <c r="F27" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G27" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="L27" t="s">
+        <v>187</v>
+      </c>
+      <c r="M27" t="s">
+        <v>188</v>
+      </c>
+      <c r="N27" t="s">
         <v>182</v>
-      </c>
-      <c r="L27" t="s">
-        <v>183</v>
-      </c>
-      <c r="M27" t="s">
-        <v>184</v>
-      </c>
-      <c r="N27" t="s">
-        <v>178</v>
       </c>
       <c r="O27" t="s">
         <v>12</v>
@@ -3025,13 +3370,13 @@
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D28" s="25">
         <v>28</v>
@@ -3040,25 +3385,25 @@
         <v>1774</v>
       </c>
       <c r="F28" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G28" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="L28" t="s">
+        <v>193</v>
+      </c>
+      <c r="M28" t="s">
+        <v>194</v>
+      </c>
+      <c r="N28" t="s">
         <v>189</v>
-      </c>
-      <c r="M28" t="s">
-        <v>190</v>
-      </c>
-      <c r="N28" t="s">
-        <v>185</v>
       </c>
       <c r="O28" t="s">
         <v>12</v>
@@ -3066,13 +3411,13 @@
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D29" s="25">
         <v>28</v>
@@ -3081,25 +3426,25 @@
         <v>1774</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G29" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29" s="8" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="L29" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M29" t="s">
+        <v>200</v>
+      </c>
+      <c r="N29" t="s">
         <v>196</v>
-      </c>
-      <c r="N29" t="s">
-        <v>192</v>
       </c>
       <c r="O29" t="s">
         <v>12</v>
@@ -3107,13 +3452,13 @@
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D30" s="25">
         <v>32</v>
@@ -3122,25 +3467,25 @@
         <v>1774</v>
       </c>
       <c r="F30" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G30" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30" s="8" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="L30" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M30" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="N30" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="O30" t="s">
         <v>12</v>
@@ -3148,13 +3493,13 @@
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D31" s="25">
         <v>32</v>
@@ -3163,25 +3508,25 @@
         <v>1774</v>
       </c>
       <c r="F31" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="G31" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31" s="8" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="L31" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="M31" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="N31" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="O31" t="s">
         <v>12</v>
@@ -3189,13 +3534,13 @@
     </row>
     <row r="32" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D32" s="25">
         <v>32</v>
@@ -3204,25 +3549,25 @@
         <v>1774</v>
       </c>
       <c r="F32" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="G32" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32" s="8" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="L32" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="M32" t="s">
+        <v>219</v>
+      </c>
+      <c r="N32" t="s">
         <v>215</v>
-      </c>
-      <c r="N32" t="s">
-        <v>211</v>
       </c>
       <c r="O32" t="s">
         <v>12</v>
@@ -3230,13 +3575,13 @@
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D33" s="25">
         <v>32</v>
@@ -3245,25 +3590,25 @@
         <v>1774</v>
       </c>
       <c r="F33" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G33" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33" s="8" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="L33" t="s">
+        <v>225</v>
+      </c>
+      <c r="M33" t="s">
+        <v>226</v>
+      </c>
+      <c r="N33" t="s">
         <v>221</v>
-      </c>
-      <c r="M33" t="s">
-        <v>222</v>
-      </c>
-      <c r="N33" t="s">
-        <v>217</v>
       </c>
       <c r="O33" t="s">
         <v>12</v>
@@ -3271,13 +3616,13 @@
     </row>
     <row r="34" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D34" s="25">
         <v>32</v>
@@ -3286,25 +3631,25 @@
         <v>1774</v>
       </c>
       <c r="F34" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G34" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34" s="8" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="L34" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="M34" t="s">
+        <v>232</v>
+      </c>
+      <c r="N34" t="s">
         <v>228</v>
-      </c>
-      <c r="N34" t="s">
-        <v>224</v>
       </c>
       <c r="O34" t="s">
         <v>12</v>
@@ -3312,13 +3657,13 @@
     </row>
     <row r="35" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D35" s="25">
         <v>32</v>
@@ -3327,25 +3672,25 @@
         <v>1774</v>
       </c>
       <c r="F35" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G35" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35" s="8" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="L35" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="M35" t="s">
+        <v>238</v>
+      </c>
+      <c r="N35" t="s">
         <v>234</v>
-      </c>
-      <c r="N35" t="s">
-        <v>230</v>
       </c>
       <c r="O35" t="s">
         <v>12</v>
@@ -3353,40 +3698,40 @@
     </row>
     <row r="36" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E36">
         <v>1774</v>
       </c>
       <c r="F36" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="G36" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36" s="8" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="L36" t="s">
+        <v>244</v>
+      </c>
+      <c r="M36" t="s">
+        <v>245</v>
+      </c>
+      <c r="N36" t="s">
         <v>240</v>
-      </c>
-      <c r="M36" t="s">
-        <v>241</v>
-      </c>
-      <c r="N36" t="s">
-        <v>236</v>
       </c>
       <c r="O36" t="s">
         <v>12</v>
@@ -3394,40 +3739,40 @@
     </row>
     <row r="37" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E37">
         <v>1775</v>
       </c>
       <c r="F37" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G37" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37" s="8" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="L37" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="M37" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="N37" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="O37" t="s">
         <v>12</v>
@@ -3435,13 +3780,13 @@
     </row>
     <row r="38" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D38" s="25">
         <v>34</v>
@@ -3450,25 +3795,25 @@
         <v>1775</v>
       </c>
       <c r="F38" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="G38" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38" s="7" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="L38" t="s">
+        <v>265</v>
+      </c>
+      <c r="M38" t="s">
+        <v>266</v>
+      </c>
+      <c r="N38" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="M38" t="s">
-        <v>262</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="O38" t="s">
         <v>12</v>
@@ -3476,13 +3821,13 @@
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D39" s="25">
         <v>34</v>
@@ -3491,25 +3836,25 @@
         <v>1775</v>
       </c>
       <c r="F39" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G39" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39" s="8" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="L39" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="M39" t="s">
+        <v>272</v>
+      </c>
+      <c r="N39" t="s">
         <v>268</v>
-      </c>
-      <c r="N39" t="s">
-        <v>264</v>
       </c>
       <c r="O39" t="s">
         <v>12</v>
@@ -3517,13 +3862,13 @@
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D40" s="25">
         <v>34</v>
@@ -3532,25 +3877,25 @@
         <v>1775</v>
       </c>
       <c r="F40" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="G40" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40" s="8" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="L40" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="M40" t="s">
+        <v>278</v>
+      </c>
+      <c r="N40" t="s">
         <v>274</v>
-      </c>
-      <c r="N40" t="s">
-        <v>270</v>
       </c>
       <c r="O40" t="s">
         <v>12</v>
@@ -3558,13 +3903,13 @@
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D41" s="25">
         <v>34</v>
@@ -3573,25 +3918,25 @@
         <v>1775</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
       <c r="K41" s="8" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="L41" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M41" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="N41" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="O41" t="s">
         <v>12</v>
@@ -3599,13 +3944,13 @@
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D42" s="25">
         <v>34</v>
@@ -3614,25 +3959,25 @@
         <v>1775</v>
       </c>
       <c r="F42" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G42" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42" s="8" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="L42" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="M42" t="s">
+        <v>287</v>
+      </c>
+      <c r="N42" t="s">
         <v>283</v>
-      </c>
-      <c r="N42" t="s">
-        <v>279</v>
       </c>
       <c r="O42" t="s">
         <v>12</v>
@@ -3640,36 +3985,36 @@
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E43">
         <v>1775</v>
       </c>
       <c r="F43" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="G43" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43" s="8" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="O43" t="s">
         <v>12</v>
@@ -3677,16 +4022,16 @@
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E44"/>
       <c r="G44"/>
@@ -3695,23 +4040,23 @@
       <c r="J44"/>
       <c r="K44" s="8"/>
       <c r="L44" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M44" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="N44"/>
       <c r="O44"/>
     </row>
     <row r="45" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C45" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D45" s="25">
         <v>43</v>
@@ -3720,25 +4065,25 @@
         <v>1777</v>
       </c>
       <c r="F45" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="G45" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
       <c r="K45" s="8" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="L45" t="s">
+        <v>303</v>
+      </c>
+      <c r="M45" t="s">
+        <v>304</v>
+      </c>
+      <c r="N45" t="s">
         <v>299</v>
-      </c>
-      <c r="M45" t="s">
-        <v>300</v>
-      </c>
-      <c r="N45" t="s">
-        <v>295</v>
       </c>
       <c r="O45" t="s">
         <v>12</v>
@@ -3746,13 +4091,13 @@
     </row>
     <row r="46" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s">
         <v>306</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" t="s">
-        <v>302</v>
       </c>
       <c r="D46" s="25">
         <v>43</v>
@@ -3761,25 +4106,25 @@
         <v>1777</v>
       </c>
       <c r="F46" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="G46" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
       <c r="K46" s="8" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="L46" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="M46" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="N46" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="O46" t="s">
         <v>12</v>
@@ -3787,13 +4132,13 @@
     </row>
     <row r="47" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D47" s="25">
         <v>43</v>
@@ -3802,25 +4147,25 @@
         <v>1777</v>
       </c>
       <c r="F47" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="G47" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
       <c r="K47" s="8" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="L47" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="M47" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="N47" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="O47" t="s">
         <v>12</v>
@@ -3828,13 +4173,13 @@
     </row>
     <row r="48" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C48" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D48" s="25">
         <v>43</v>
@@ -3843,25 +4188,25 @@
         <v>1777</v>
       </c>
       <c r="F48" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="G48" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
       <c r="K48" s="8" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="L48" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="M48" t="s">
+        <v>321</v>
+      </c>
+      <c r="N48" t="s">
         <v>317</v>
-      </c>
-      <c r="N48" t="s">
-        <v>313</v>
       </c>
       <c r="O48" t="s">
         <v>12</v>
@@ -3869,13 +4214,13 @@
     </row>
     <row r="49" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D49" s="25">
         <v>43</v>
@@ -3884,25 +4229,25 @@
         <v>1777</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
       <c r="K49" s="8" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L49" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="M49" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="N49" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="O49" t="s">
         <v>12</v>
@@ -3910,13 +4255,13 @@
     </row>
     <row r="50" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D50" s="25">
         <v>43</v>
@@ -3925,10 +4270,10 @@
         <v>1777</v>
       </c>
       <c r="F50" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="G50" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="H50"/>
       <c r="I50"/>
@@ -3937,7 +4282,7 @@
       <c r="L50"/>
       <c r="M50"/>
       <c r="N50" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="O50" t="s">
         <v>12</v>
@@ -3945,13 +4290,13 @@
     </row>
     <row r="51" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
         <v>331</v>
-      </c>
-      <c r="B51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" t="s">
-        <v>327</v>
       </c>
       <c r="D51" s="25">
         <v>55</v>
@@ -3960,25 +4305,25 @@
         <v>1779</v>
       </c>
       <c r="F51" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="G51" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
       <c r="K51" s="8" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="L51" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="M51" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="N51" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="O51" t="s">
         <v>12</v>
@@ -3986,13 +4331,13 @@
     </row>
     <row r="52" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D52" s="25">
         <v>55</v>
@@ -4001,10 +4346,10 @@
         <v>1779</v>
       </c>
       <c r="F52" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="G52" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="H52"/>
       <c r="I52"/>
@@ -4013,13 +4358,13 @@
         <v>35510</v>
       </c>
       <c r="L52" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M52" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="O52" t="s">
         <v>12</v>
@@ -4027,13 +4372,13 @@
     </row>
     <row r="53" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D53" s="25">
         <v>55</v>
@@ -4042,25 +4387,25 @@
         <v>1779</v>
       </c>
       <c r="F53" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="G53" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L53" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="M53" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="N53" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O53" t="s">
         <v>12</v>
@@ -4068,13 +4413,13 @@
     </row>
     <row r="54" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D54" s="25">
         <v>55</v>
@@ -4083,25 +4428,25 @@
         <v>1779</v>
       </c>
       <c r="F54" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="G54" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54" s="8" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="L54" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="M54" t="s">
+        <v>351</v>
+      </c>
+      <c r="N54" t="s">
         <v>347</v>
-      </c>
-      <c r="N54" t="s">
-        <v>343</v>
       </c>
       <c r="O54" t="s">
         <v>12</v>
@@ -4109,13 +4454,13 @@
     </row>
     <row r="55" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B55" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C55" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D55" s="25">
         <v>55</v>
@@ -4124,25 +4469,25 @@
         <v>1779</v>
       </c>
       <c r="F55" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="G55" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55" s="7" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="L55" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M55" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="O55" t="s">
         <v>12</v>
@@ -4150,13 +4495,13 @@
     </row>
     <row r="56" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D56" s="25">
         <v>55</v>
@@ -4165,25 +4510,25 @@
         <v>1779</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G56" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
       <c r="K56" s="8" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="L56" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="M56" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="N56" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="O56" t="s">
         <v>12</v>
@@ -4191,46 +4536,46 @@
     </row>
     <row r="57" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="E57">
         <v>1792</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
       <c r="K57" s="8"/>
       <c r="L57" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="M57" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="N57"/>
       <c r="O57"/>
     </row>
     <row r="58" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D58" s="25">
         <v>112</v>
@@ -4239,25 +4584,25 @@
         <v>1792</v>
       </c>
       <c r="F58" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="G58" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="H58"/>
       <c r="I58"/>
       <c r="J58"/>
       <c r="K58" s="8" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="L58" t="s">
+        <v>371</v>
+      </c>
+      <c r="M58" t="s">
+        <v>372</v>
+      </c>
+      <c r="N58" t="s">
         <v>367</v>
-      </c>
-      <c r="M58" t="s">
-        <v>368</v>
-      </c>
-      <c r="N58" t="s">
-        <v>363</v>
       </c>
       <c r="O58" t="s">
         <v>12</v>
@@ -4265,13 +4610,13 @@
     </row>
     <row r="59" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D59" s="25">
         <v>112</v>
@@ -4280,25 +4625,25 @@
         <v>1792</v>
       </c>
       <c r="F59" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="G59" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="H59"/>
       <c r="I59"/>
       <c r="J59"/>
       <c r="K59" s="8" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="L59" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M59" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N59" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="O59" t="s">
         <v>12</v>
@@ -4306,13 +4651,13 @@
     </row>
     <row r="60" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D60" s="25">
         <v>112</v>
@@ -4321,36 +4666,36 @@
         <v>1792</v>
       </c>
       <c r="F60" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="G60" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60"/>
       <c r="K60" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="M60" t="s">
+        <v>383</v>
+      </c>
+      <c r="N60" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="M60" t="s">
+      <c r="O60" t="s">
         <v>379</v>
-      </c>
-      <c r="N60" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="O60" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="61" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C61" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D61" s="25">
         <v>112</v>
@@ -4359,25 +4704,25 @@
         <v>1792</v>
       </c>
       <c r="F61" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="G61" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61"/>
       <c r="K61" s="8" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="L61" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="M61" t="s">
+        <v>389</v>
+      </c>
+      <c r="N61" t="s">
         <v>385</v>
-      </c>
-      <c r="N61" t="s">
-        <v>381</v>
       </c>
       <c r="O61" t="s">
         <v>12</v>
@@ -4385,13 +4730,13 @@
     </row>
     <row r="62" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C62" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D62" s="25">
         <v>112</v>
@@ -4400,25 +4745,25 @@
         <v>1792</v>
       </c>
       <c r="F62" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="G62" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62"/>
       <c r="K62" s="7" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="L62" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="M62" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="O62" t="s">
         <v>13</v>
@@ -4426,40 +4771,40 @@
     </row>
     <row r="63" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C63" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E63">
         <v>1792</v>
       </c>
       <c r="F63" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="G63" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
       <c r="K63" s="7" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="L63" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M63" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="O63" t="s">
         <v>12</v>
@@ -4467,13 +4812,13 @@
     </row>
     <row r="64" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D64" s="25">
         <v>113</v>
@@ -4482,25 +4827,25 @@
         <v>1792</v>
       </c>
       <c r="F64" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="G64" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
       <c r="K64" s="8" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="L64" t="s">
+        <v>410</v>
+      </c>
+      <c r="M64" t="s">
+        <v>411</v>
+      </c>
+      <c r="N64" s="3" t="s">
         <v>406</v>
-      </c>
-      <c r="M64" t="s">
-        <v>407</v>
-      </c>
-      <c r="N64" s="3" t="s">
-        <v>402</v>
       </c>
       <c r="O64" t="s">
         <v>12</v>
@@ -4508,13 +4853,13 @@
     </row>
     <row r="65" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B65" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C65" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D65" s="25">
         <v>113</v>
@@ -4523,25 +4868,25 @@
         <v>1792</v>
       </c>
       <c r="F65" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="G65" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="H65"/>
       <c r="I65"/>
       <c r="J65"/>
       <c r="K65" s="7" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="L65" t="s">
+        <v>417</v>
+      </c>
+      <c r="M65" t="s">
+        <v>418</v>
+      </c>
+      <c r="N65" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="M65" t="s">
-        <v>414</v>
-      </c>
-      <c r="N65" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="O65" t="s">
         <v>12</v>
@@ -4549,13 +4894,13 @@
     </row>
     <row r="66" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D66" s="25">
         <v>113</v>
@@ -4564,25 +4909,25 @@
         <v>1792</v>
       </c>
       <c r="F66" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="G66" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="H66"/>
       <c r="I66"/>
       <c r="J66"/>
       <c r="K66" s="7" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="L66" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="M66" t="s">
+        <v>424</v>
+      </c>
+      <c r="N66" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="N66" s="3" t="s">
-        <v>416</v>
       </c>
       <c r="O66" t="s">
         <v>12</v>
@@ -4590,13 +4935,13 @@
     </row>
     <row r="67" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B67" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D67" s="25">
         <v>113</v>
@@ -4605,37 +4950,37 @@
         <v>1792</v>
       </c>
       <c r="F67" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="G67" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="H67"/>
       <c r="I67"/>
       <c r="J67"/>
       <c r="K67" s="7" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="L67" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="M67" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="O67"/>
     </row>
     <row r="68" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C68" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D68" s="25">
         <v>113</v>
@@ -4644,25 +4989,25 @@
         <v>1792</v>
       </c>
       <c r="F68" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="G68" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="H68"/>
       <c r="I68"/>
       <c r="J68"/>
       <c r="K68" s="7" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="L68" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="M68" t="s">
+        <v>435</v>
+      </c>
+      <c r="N68" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="N68" s="3" t="s">
-        <v>427</v>
       </c>
       <c r="O68" t="s">
         <v>12</v>
@@ -4670,13 +5015,13 @@
     </row>
     <row r="69" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C69" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D69" s="25">
         <v>113</v>
@@ -4685,25 +5030,25 @@
         <v>1792</v>
       </c>
       <c r="F69" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="G69" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="H69"/>
       <c r="I69"/>
       <c r="J69"/>
       <c r="K69" s="7" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="L69" t="s">
+        <v>441</v>
+      </c>
+      <c r="M69" t="s">
+        <v>442</v>
+      </c>
+      <c r="N69" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="M69" t="s">
-        <v>438</v>
-      </c>
-      <c r="N69" s="3" t="s">
-        <v>433</v>
       </c>
       <c r="O69" t="s">
         <v>12</v>
@@ -4711,13 +5056,13 @@
     </row>
     <row r="70" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B70" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D70" s="25">
         <v>113</v>
@@ -4726,301 +5071,699 @@
         <v>1793</v>
       </c>
       <c r="F70" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="G70" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="H70"/>
       <c r="I70"/>
       <c r="J70"/>
       <c r="K70" s="7" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="L70" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="M70" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="O70" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71" s="25"/>
-      <c r="E71"/>
+      <c r="A71" s="27" t="s">
+        <v>453</v>
+      </c>
+      <c r="B71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C71" t="s">
+        <v>451</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="E71">
+        <v>1794</v>
+      </c>
       <c r="F71"/>
-      <c r="G71"/>
+      <c r="G71" t="s">
+        <v>449</v>
+      </c>
       <c r="H71"/>
       <c r="I71"/>
       <c r="J71"/>
       <c r="K71" s="7"/>
-      <c r="L71" s="18"/>
-      <c r="M71" s="18"/>
+      <c r="L71" s="18" t="s">
+        <v>454</v>
+      </c>
+      <c r="M71" s="18" t="s">
+        <v>455</v>
+      </c>
       <c r="N71" s="7"/>
       <c r="O71"/>
     </row>
     <row r="72" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72" s="25"/>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
+      <c r="A72" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="B72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" t="s">
+        <v>450</v>
+      </c>
+      <c r="D72" s="25">
+        <v>121</v>
+      </c>
+      <c r="E72">
+        <v>1794</v>
+      </c>
+      <c r="F72" t="s">
+        <v>459</v>
+      </c>
+      <c r="G72" t="s">
+        <v>459</v>
+      </c>
       <c r="H72"/>
       <c r="I72"/>
       <c r="J72"/>
       <c r="K72"/>
-      <c r="L72"/>
-      <c r="M72"/>
-      <c r="N72"/>
+      <c r="L72" t="s">
+        <v>457</v>
+      </c>
+      <c r="M72" t="s">
+        <v>422</v>
+      </c>
+      <c r="N72" s="3" t="s">
+        <v>456</v>
+      </c>
       <c r="O72"/>
     </row>
     <row r="73" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73" s="25"/>
-      <c r="E73"/>
-      <c r="F73"/>
-      <c r="G73"/>
+      <c r="A73" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="B73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" t="s">
+        <v>450</v>
+      </c>
+      <c r="D73" s="25">
+        <v>121</v>
+      </c>
+      <c r="E73">
+        <v>1794</v>
+      </c>
+      <c r="F73" t="s">
+        <v>462</v>
+      </c>
+      <c r="G73" t="s">
+        <v>463</v>
+      </c>
       <c r="H73"/>
       <c r="I73"/>
       <c r="J73"/>
-      <c r="K73"/>
-      <c r="L73"/>
-      <c r="M73"/>
-      <c r="N73"/>
-      <c r="O73"/>
+      <c r="K73" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="L73" t="s">
+        <v>464</v>
+      </c>
+      <c r="M73" t="s">
+        <v>16</v>
+      </c>
+      <c r="N73" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="O73" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="74" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="D74" s="25"/>
-      <c r="E74"/>
-      <c r="F74"/>
-      <c r="G74"/>
+      <c r="A74" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" t="s">
+        <v>450</v>
+      </c>
+      <c r="D74" s="25">
+        <v>121</v>
+      </c>
+      <c r="E74">
+        <v>1794</v>
+      </c>
+      <c r="F74" t="s">
+        <v>466</v>
+      </c>
+      <c r="G74" t="s">
+        <v>468</v>
+      </c>
       <c r="H74"/>
       <c r="I74"/>
       <c r="J74"/>
-      <c r="K74"/>
-      <c r="L74"/>
-      <c r="M74"/>
-      <c r="N74"/>
-      <c r="O74"/>
+      <c r="K74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L74" t="s">
+        <v>470</v>
+      </c>
+      <c r="M74" t="s">
+        <v>471</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="O74" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="75" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="D75" s="25"/>
-      <c r="E75"/>
-      <c r="F75"/>
-      <c r="G75"/>
+      <c r="A75" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" t="s">
+        <v>450</v>
+      </c>
+      <c r="D75" s="25">
+        <v>121</v>
+      </c>
+      <c r="E75">
+        <v>1794</v>
+      </c>
+      <c r="F75" t="s">
+        <v>474</v>
+      </c>
+      <c r="G75" t="s">
+        <v>475</v>
+      </c>
       <c r="H75"/>
       <c r="I75"/>
       <c r="J75"/>
-      <c r="K75"/>
-      <c r="L75"/>
-      <c r="M75"/>
-      <c r="N75"/>
-      <c r="O75"/>
+      <c r="K75" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="L75" t="s">
+        <v>476</v>
+      </c>
+      <c r="M75" t="s">
+        <v>42</v>
+      </c>
+      <c r="N75" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="O75" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="76" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="D76" s="25"/>
-      <c r="E76"/>
-      <c r="F76"/>
-      <c r="G76"/>
+      <c r="A76" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="B76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" t="s">
+        <v>450</v>
+      </c>
+      <c r="D76" s="25">
+        <v>121</v>
+      </c>
+      <c r="E76">
+        <v>1794</v>
+      </c>
+      <c r="F76" t="s">
+        <v>427</v>
+      </c>
+      <c r="G76" t="s">
+        <v>428</v>
+      </c>
       <c r="H76"/>
       <c r="I76"/>
       <c r="J76"/>
-      <c r="K76"/>
-      <c r="L76"/>
-      <c r="M76"/>
-      <c r="N76"/>
+      <c r="K76" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="L76" t="s">
+        <v>478</v>
+      </c>
+      <c r="M76" t="s">
+        <v>479</v>
+      </c>
+      <c r="N76" s="3" t="s">
+        <v>477</v>
+      </c>
       <c r="O76"/>
     </row>
     <row r="77" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="D77" s="25"/>
-      <c r="E77"/>
-      <c r="F77"/>
-      <c r="G77"/>
+      <c r="A77" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="B77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" t="s">
+        <v>450</v>
+      </c>
+      <c r="D77" s="25">
+        <v>121</v>
+      </c>
+      <c r="E77">
+        <v>1794</v>
+      </c>
+      <c r="F77" t="s">
+        <v>482</v>
+      </c>
+      <c r="G77" t="s">
+        <v>483</v>
+      </c>
       <c r="H77"/>
       <c r="I77"/>
       <c r="J77"/>
-      <c r="K77"/>
-      <c r="L77"/>
-      <c r="M77"/>
-      <c r="N77"/>
-      <c r="O77"/>
+      <c r="K77" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="L77" t="s">
+        <v>485</v>
+      </c>
+      <c r="M77" t="s">
+        <v>486</v>
+      </c>
+      <c r="N77" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="O77" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="78" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="D78" s="25"/>
-      <c r="E78"/>
-      <c r="F78"/>
-      <c r="G78"/>
+      <c r="A78" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" t="s">
+        <v>450</v>
+      </c>
+      <c r="D78" s="25">
+        <v>121</v>
+      </c>
+      <c r="E78">
+        <v>1794</v>
+      </c>
+      <c r="F78" t="s">
+        <v>489</v>
+      </c>
+      <c r="G78" t="s">
+        <v>490</v>
+      </c>
       <c r="H78"/>
       <c r="I78"/>
       <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78"/>
-      <c r="M78"/>
-      <c r="N78"/>
-      <c r="O78"/>
+      <c r="K78" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="L78" t="s">
+        <v>429</v>
+      </c>
+      <c r="M78" t="s">
+        <v>491</v>
+      </c>
+      <c r="N78" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="O78" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="79" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="D79" s="25"/>
-      <c r="E79"/>
-      <c r="F79"/>
-      <c r="G79"/>
+      <c r="A79" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" t="s">
+        <v>450</v>
+      </c>
+      <c r="D79" s="25">
+        <v>121</v>
+      </c>
+      <c r="E79">
+        <v>1794</v>
+      </c>
+      <c r="F79" t="s">
+        <v>494</v>
+      </c>
+      <c r="G79" t="s">
+        <v>495</v>
+      </c>
       <c r="H79"/>
       <c r="I79"/>
       <c r="J79"/>
-      <c r="K79"/>
-      <c r="L79"/>
-      <c r="M79"/>
-      <c r="N79"/>
-      <c r="O79"/>
+      <c r="K79" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="L79" t="s">
+        <v>497</v>
+      </c>
+      <c r="M79" t="s">
+        <v>498</v>
+      </c>
+      <c r="N79" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="O79" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="80" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80" s="25"/>
-      <c r="E80"/>
-      <c r="F80"/>
-      <c r="G80"/>
-      <c r="H80"/>
-      <c r="I80"/>
+      <c r="A80" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="B80" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" t="s">
+        <v>500</v>
+      </c>
+      <c r="D80" s="25">
+        <v>156</v>
+      </c>
+      <c r="E80">
+        <v>1801</v>
+      </c>
+      <c r="F80" t="s">
+        <v>508</v>
+      </c>
+      <c r="G80" t="s">
+        <v>509</v>
+      </c>
+      <c r="H80" t="s">
+        <v>506</v>
+      </c>
+      <c r="I80" t="s">
+        <v>507</v>
+      </c>
       <c r="J80"/>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80"/>
-      <c r="N80"/>
-      <c r="O80"/>
+      <c r="K80" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="L80" t="s">
+        <v>504</v>
+      </c>
+      <c r="M80" t="s">
+        <v>505</v>
+      </c>
+      <c r="N80" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="O80" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="81" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81" s="25"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
+      <c r="A81" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="B81" t="s">
+        <v>27</v>
+      </c>
+      <c r="C81" t="s">
+        <v>500</v>
+      </c>
+      <c r="D81" s="25">
+        <v>156</v>
+      </c>
+      <c r="E81">
+        <v>1801</v>
+      </c>
+      <c r="F81" t="s">
+        <v>516</v>
+      </c>
+      <c r="G81" t="s">
+        <v>517</v>
+      </c>
+      <c r="H81" t="s">
+        <v>514</v>
+      </c>
+      <c r="I81" t="s">
+        <v>515</v>
+      </c>
       <c r="J81"/>
-      <c r="K81"/>
-      <c r="L81"/>
-      <c r="M81"/>
-      <c r="N81"/>
-      <c r="O81"/>
+      <c r="K81" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L81" t="s">
+        <v>513</v>
+      </c>
+      <c r="M81" t="s">
+        <v>512</v>
+      </c>
+      <c r="N81" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="O81" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="82" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82" s="25"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
+      <c r="A82" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="B82" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" t="s">
+        <v>500</v>
+      </c>
+      <c r="D82" s="25">
+        <v>156</v>
+      </c>
+      <c r="E82">
+        <v>1801</v>
+      </c>
+      <c r="F82" t="s">
+        <v>523</v>
+      </c>
+      <c r="G82" t="s">
+        <v>525</v>
+      </c>
+      <c r="H82" t="s">
+        <v>522</v>
+      </c>
+      <c r="I82" t="s">
+        <v>524</v>
+      </c>
       <c r="J82"/>
-      <c r="K82"/>
-      <c r="L82"/>
-      <c r="M82"/>
-      <c r="N82"/>
-      <c r="O82"/>
+      <c r="K82" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="L82" t="s">
+        <v>520</v>
+      </c>
+      <c r="M82" t="s">
+        <v>521</v>
+      </c>
+      <c r="N82" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="O82" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="83" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="D83" s="25"/>
-      <c r="E83"/>
-      <c r="F83"/>
-      <c r="G83"/>
-      <c r="H83"/>
-      <c r="I83"/>
+      <c r="A83" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="B83" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" t="s">
+        <v>500</v>
+      </c>
+      <c r="D83" s="25">
+        <v>156</v>
+      </c>
+      <c r="E83">
+        <v>1801</v>
+      </c>
+      <c r="F83" t="s">
+        <v>532</v>
+      </c>
+      <c r="G83" t="s">
+        <v>534</v>
+      </c>
+      <c r="H83" t="s">
+        <v>531</v>
+      </c>
+      <c r="I83" t="s">
+        <v>533</v>
+      </c>
       <c r="J83"/>
-      <c r="K83"/>
-      <c r="L83"/>
-      <c r="M83"/>
-      <c r="N83"/>
-      <c r="O83"/>
+      <c r="K83" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="L83" t="s">
+        <v>529</v>
+      </c>
+      <c r="M83" t="s">
+        <v>530</v>
+      </c>
+      <c r="N83" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="O83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="84" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84" s="25"/>
-      <c r="E84"/>
-      <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84"/>
-      <c r="I84"/>
+      <c r="A84" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="B84" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84" t="s">
+        <v>500</v>
+      </c>
+      <c r="D84" s="25">
+        <v>156</v>
+      </c>
+      <c r="E84">
+        <v>1801</v>
+      </c>
+      <c r="F84" t="s">
+        <v>541</v>
+      </c>
+      <c r="G84" t="s">
+        <v>542</v>
+      </c>
+      <c r="H84" t="s">
+        <v>539</v>
+      </c>
+      <c r="I84" t="s">
+        <v>540</v>
+      </c>
       <c r="J84"/>
-      <c r="K84" s="19"/>
-      <c r="L84"/>
-      <c r="M84"/>
-      <c r="N84" s="7"/>
-      <c r="O84"/>
+      <c r="K84" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="L84" t="s">
+        <v>538</v>
+      </c>
+      <c r="M84" t="s">
+        <v>16</v>
+      </c>
+      <c r="N84" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="O84" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="85" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85" s="25"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
+      <c r="A85" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="B85" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" t="s">
+        <v>500</v>
+      </c>
+      <c r="D85" s="25">
+        <v>156</v>
+      </c>
+      <c r="E85">
+        <v>1801</v>
+      </c>
+      <c r="F85" t="s">
+        <v>550</v>
+      </c>
+      <c r="G85" t="s">
+        <v>549</v>
+      </c>
+      <c r="H85" t="s">
+        <v>547</v>
+      </c>
+      <c r="I85" t="s">
+        <v>548</v>
+      </c>
       <c r="J85"/>
-      <c r="K85"/>
-      <c r="L85"/>
-      <c r="M85"/>
-      <c r="N85"/>
-      <c r="O85"/>
+      <c r="K85" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="L85" t="s">
+        <v>546</v>
+      </c>
+      <c r="M85" t="s">
+        <v>495</v>
+      </c>
+      <c r="N85" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="O85" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="86" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
-      <c r="B86"/>
-      <c r="C86"/>
-      <c r="D86" s="25"/>
-      <c r="E86"/>
-      <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
+      <c r="A86" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="B86" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86" t="s">
+        <v>500</v>
+      </c>
+      <c r="D86" s="25">
+        <v>156</v>
+      </c>
+      <c r="E86">
+        <v>1801</v>
+      </c>
+      <c r="F86" t="s">
+        <v>553</v>
+      </c>
+      <c r="G86" t="s">
+        <v>554</v>
+      </c>
+      <c r="H86" t="s">
+        <v>558</v>
+      </c>
+      <c r="I86" t="s">
+        <v>559</v>
+      </c>
       <c r="J86"/>
-      <c r="K86"/>
-      <c r="L86"/>
-      <c r="M86"/>
-      <c r="N86"/>
-      <c r="O86"/>
+      <c r="K86" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="L86" t="s">
+        <v>556</v>
+      </c>
+      <c r="M86" t="s">
+        <v>557</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="O86" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="87" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>

</xml_diff>

<commit_message>
Afegint dades de llibres
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Baptismes/Excel/Index_llibres_Baptismes.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Baptismes/Excel/Index_llibres_Baptismes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Baptismes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA5CC48-42A9-45B3-A6BA-867E33F8D912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E9D809-35CC-4088-BC18-D428F388A601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baptismes" sheetId="2" r:id="rId1"/>
@@ -5333,8 +5333,8 @@
   <dimension ref="A1:Q17820"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18133" sqref="F18133"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>